<commit_message>
Added ui of date picker.
</commit_message>
<xml_diff>
--- a/pages/registration/assets/documents/MCIExcelTemplate.xlsx
+++ b/pages/registration/assets/documents/MCIExcelTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imohammadsadra/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imohammadsadra/Downloads/Bazidid/pages/registration/assets/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AFB8A2-7E68-D349-ACD3-D84D1FD4C747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF2E9C1-BE50-604B-90BC-B8F85EA8D43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="اسامی دانش‌آموزان و مربیان" sheetId="1" r:id="rId1"/>
@@ -334,10 +334,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -362,29 +358,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <font>
         <strike val="0"/>
@@ -397,6 +397,7 @@
         <name val="B Nazanin"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -410,6 +411,7 @@
         <name val="B Nazanin"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -423,6 +425,14 @@
         <name val="B Nazanin"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color rgb="FFC5CAE9"/>
+        </right>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -454,8 +464,8 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="اسامی دانش‌آموزان و مربیان-style" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="5"/>
-      <tableStyleElement type="secondRowStripe" dxfId="4"/>
+      <tableStyleElement type="firstRowStripe" dxfId="6"/>
+      <tableStyleElement type="secondRowStripe" dxfId="5"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -529,8 +539,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:F22" headerRowCount="0">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6" dataDxfId="0"/>
@@ -845,13 +855,13 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="13" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="11" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" customWidth="1"/>
@@ -860,28 +870,28 @@
   <sheetData>
     <row r="1" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="9"/>
+      <c r="B1" s="19"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-    </row>
-    <row r="2" spans="1:6" s="18" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="15" t="e">
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="12"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="13" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>3</v>
       </c>
     </row>
@@ -889,23 +899,23 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="24"/>
+      <c r="D4" s="22"/>
       <c r="E4" s="25"/>
       <c r="F4" s="26"/>
     </row>
@@ -913,221 +923,221 @@
       <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>2</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24"/>
     </row>
     <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>3</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
     </row>
     <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>4</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
     </row>
     <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>5</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>6</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
     </row>
     <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>7</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
     </row>
     <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>8</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24"/>
     </row>
     <row r="13" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>9</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="21"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="24"/>
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>10</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>11</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="21"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>12</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="24"/>
     </row>
     <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>13</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="21"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>14</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
     </row>
     <row r="19" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>15</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="21"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
     </row>
     <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>16</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="21"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>17</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="21"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>18</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:6" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="7"/>
-      <c r="B23" s="11"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="4"/>
       <c r="D23" s="5">
         <f t="shared" ref="D23:F23" si="0">COUNTIF($C23,D$2)</f>
@@ -1154,7 +1164,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showDropDown="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Attendance key'!#REF!</xm:f>

</xml_diff>